<commit_message>
Make display clip left
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -461,7 +461,7 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>41.220999999999997</v>
+        <v>553.24400000000003</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -484,15 +484,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-370.65899999999999</v>
+        <v>479.56700000000001</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -504,15 +504,15 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>-208.08</v>
+        <v>370.19200000000001</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -524,7 +524,7 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>561.20699999999999</v>
+        <v>-226.65700000000001</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
@@ -544,15 +544,15 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-913.51300000000003</v>
+        <v>-843.52300000000002</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -564,21 +564,21 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>-838.43</v>
+        <v>-153.51300000000001</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
     </row>
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>-910.14499999999998</v>
+        <v>634.70600000000002</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -586,43 +586,43 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.94499999999999995</v>
+        <v>0.28199999999999997</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">VLOOKUP(B10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>872.81899999999996</v>
+        <v>179.04300000000001</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(E10,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>10.349</v>
+        <v>-772.17</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>28.826000000000001</v>
+        <v>-713.27700000000004</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -634,19 +634,19 @@
       </c>
       <c r="M10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-248.05699999999999</v>
+        <v>153.036</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O10" t="str">
         <f ca="1">VLOOKUP(N10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-287.67399999999998</v>
+        <v>558.28899999999999</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -658,37 +658,37 @@
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>688.21</v>
+        <v>633.58299999999997</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.88800000000000001</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:C19" ca="1" si="5">VLOOKUP(B11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-831.58500000000004</v>
+        <v>-915.35400000000004</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>26.164999999999999</v>
+        <v>237.804</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
@@ -700,73 +700,73 @@
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-54.104999999999997</v>
+        <v>-454.90899999999999</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:L19" ca="1" si="14">VLOOKUP(K11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="M11">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>635.89300000000003</v>
+        <v>536.39400000000001</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O19" ca="1" si="17">VLOOKUP(N11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-396.47300000000001</v>
+        <v>-565.10599999999999</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ref="R11:R19" ca="1" si="20">VLOOKUP(Q11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-583.84299999999996</v>
+        <v>-787.13199999999995</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.96899999999999997</v>
+        <v>0.52100000000000002</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>789.84299999999996</v>
+        <v>678.00699999999995</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>486.50799999999998</v>
+        <v>-352.00400000000002</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
@@ -778,85 +778,85 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>179.499</v>
+        <v>141.953</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="15"/>
-        <v>848.03</v>
+        <v>-866.57600000000002</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>-567.46699999999998</v>
+        <v>526.40700000000004</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>455.96600000000001</v>
+        <v>456.22300000000001</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.78200000000000003</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>-76.728999999999999</v>
+        <v>-526.76599999999996</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>-518.27099999999996</v>
+        <v>-449.25299999999999</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>-190.36799999999999</v>
+        <v>69.319999999999993</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
@@ -868,127 +868,127 @@
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="15"/>
-        <v>-738.51900000000001</v>
+        <v>160.066</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>-953.31799999999998</v>
+        <v>330.30900000000003</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>426.221</v>
+        <v>-164.953</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.58299999999999996</v>
+        <v>0.84199999999999997</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>311.88</v>
+        <v>-512.87599999999998</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>-962.97500000000002</v>
+        <v>401.95800000000003</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>574.05600000000004</v>
+        <v>-994.79</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="15"/>
-        <v>8.6389999999999993</v>
+        <v>-248.28100000000001</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>553.53300000000002</v>
+        <v>-705.24800000000005</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>-622.19000000000005</v>
+        <v>-285.846</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26800000000000002</v>
+        <v>0.52900000000000003</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>-590.74300000000005</v>
+        <v>73.02</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
@@ -1000,31 +1000,31 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>436.58300000000003</v>
+        <v>203.75200000000001</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>-752.27599999999995</v>
+        <v>368.54199999999997</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="15"/>
-        <v>-181.858</v>
+        <v>-349.75599999999997</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
@@ -1036,49 +1036,49 @@
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>306.61700000000002</v>
+        <v>-791.99900000000002</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>-169.42699999999999</v>
+        <v>226.33699999999999</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.76400000000000001</v>
+        <v>0.91300000000000003</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>274.63400000000001</v>
+        <v>-828.40700000000004</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>771.17499999999995</v>
+        <v>358.755</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
@@ -1090,85 +1090,85 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>-197.93799999999999</v>
+        <v>-5.1029999999999998</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="15"/>
-        <v>-573.976</v>
+        <v>-84.257999999999996</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>-280.14400000000001</v>
+        <v>-893.30399999999997</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>-887.79399999999998</v>
+        <v>539.01800000000003</v>
       </c>
     </row>
     <row r="17" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.71199999999999997</v>
+        <v>0.35199999999999998</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>516.25699999999995</v>
+        <v>956.99199999999996</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>-869.577</v>
+        <v>937.17399999999998</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>-177.69300000000001</v>
+        <v>175.82400000000001</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
@@ -1180,61 +1180,61 @@
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="15"/>
-        <v>566.20399999999995</v>
+        <v>-202.47399999999999</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>554.99099999999999</v>
+        <v>-822.59199999999998</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>-519.33299999999997</v>
+        <v>-652.63</v>
       </c>
     </row>
     <row r="18" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.26500000000000001</v>
+        <v>0.97799999999999998</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>383.67599999999999</v>
+        <v>235.82400000000001</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>736.39099999999996</v>
+        <v>-843.37</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>31.957000000000001</v>
+        <v>-345.77</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="15"/>
-        <v>-957.69600000000003</v>
+        <v>-368.512</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
@@ -1270,97 +1270,97 @@
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>206.321</v>
+        <v>-677.19</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>-574.83100000000002</v>
+        <v>424.37599999999998</v>
       </c>
     </row>
     <row r="19" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.92200000000000004</v>
+        <v>0.51</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>753.59699999999998</v>
+        <v>-703.50699999999995</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>-324.35500000000002</v>
+        <v>-863.71100000000001</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>559.53899999999999</v>
+        <v>718.202</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="15"/>
-        <v>-781.44399999999996</v>
+        <v>914.51199999999994</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>-372.13099999999997</v>
+        <v>-968.83399999999995</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>170.62200000000001</v>
+        <v>945.33</v>
       </c>
     </row>
     <row r="20" spans="1:25" collapsed="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Prevent wrapping of text
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C22" sqref="A22:XFD22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -461,15 +461,15 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>553.24400000000003</v>
+        <v>-447.34399999999999</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="str">
         <f ca="1">VLOOKUP(B1,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -484,15 +484,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>479.56700000000001</v>
+        <v>923.54700000000003</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -504,15 +504,15 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>370.19200000000001</v>
+        <v>-726.47199999999998</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -524,15 +524,15 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>-226.65700000000001</v>
+        <v>916.73699999999997</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -544,7 +544,7 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-843.52300000000002</v>
+        <v>-966.07799999999997</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
@@ -564,21 +564,21 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>-153.51300000000001</v>
+        <v>154.07400000000001</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
     </row>
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>634.70600000000002</v>
+        <v>740.30799999999999</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -586,43 +586,43 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.28199999999999997</v>
+        <v>0.85799999999999998</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">VLOOKUP(B10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>179.04300000000001</v>
+        <v>72.694000000000003</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(E10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-772.17</v>
+        <v>162.69399999999999</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-713.27700000000004</v>
+        <v>-541.57299999999998</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -634,7 +634,7 @@
       </c>
       <c r="M10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>153.036</v>
+        <v>-993.10299999999995</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -646,49 +646,49 @@
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>558.28899999999999</v>
+        <v>979.8</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R10" t="str">
         <f ca="1">VLOOKUP(Q10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>633.58299999999997</v>
+        <v>-982.76700000000005</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>8.3000000000000004E-2</v>
+        <v>0.94899999999999995</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:C19" ca="1" si="5">VLOOKUP(B11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-915.35400000000004</v>
+        <v>-898.56100000000004</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>237.804</v>
+        <v>-855.88199999999995</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
@@ -700,7 +700,7 @@
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-454.90899999999999</v>
+        <v>829.45</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
@@ -712,7 +712,7 @@
       </c>
       <c r="M11">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>536.39400000000001</v>
+        <v>883.173</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
@@ -724,73 +724,73 @@
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-565.10599999999999</v>
+        <v>26.739000000000001</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ref="R11:R19" ca="1" si="20">VLOOKUP(Q11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-787.13199999999995</v>
+        <v>-389.79</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52100000000000002</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>678.00699999999995</v>
+        <v>-411.267</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>-352.00400000000002</v>
+        <v>-123.19799999999999</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>141.953</v>
+        <v>505.47199999999998</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="15"/>
-        <v>-866.57600000000002</v>
+        <v>524.79</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
@@ -802,181 +802,181 @@
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>526.40700000000004</v>
+        <v>-830.83299999999997</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>456.22300000000001</v>
+        <v>-757.57500000000005</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.41199999999999998</v>
+        <v>0.40500000000000003</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>-526.76599999999996</v>
+        <v>-946.05399999999997</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>-449.25299999999999</v>
+        <v>-845.68799999999999</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>69.319999999999993</v>
+        <v>-475.28500000000003</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="15"/>
-        <v>160.066</v>
+        <v>-524.42499999999995</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>330.30900000000003</v>
+        <v>-48.222999999999999</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>-164.953</v>
+        <v>-556.00400000000002</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.84199999999999997</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>-512.87599999999998</v>
+        <v>962.678</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>401.95800000000003</v>
+        <v>538.59900000000005</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>-994.79</v>
+        <v>-61.835999999999999</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="15"/>
-        <v>-248.28100000000001</v>
+        <v>-184.00399999999999</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>-705.24800000000005</v>
+        <v>-149.11199999999999</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>-285.846</v>
+        <v>808.51499999999999</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52900000000000003</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
@@ -988,19 +988,19 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>73.02</v>
+        <v>-372.24200000000002</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>203.75200000000001</v>
+        <v>-29.215</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>368.54199999999997</v>
+        <v>-63.451000000000001</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
@@ -1024,115 +1024,115 @@
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="15"/>
-        <v>-349.75599999999997</v>
+        <v>-783.36699999999996</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>-791.99900000000002</v>
+        <v>-801.18</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>226.33699999999999</v>
+        <v>-971.82799999999997</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.91300000000000003</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>-828.40700000000004</v>
+        <v>537.93799999999999</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>358.755</v>
+        <v>61.238999999999997</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>-5.1029999999999998</v>
+        <v>-968.55</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="15"/>
-        <v>-84.257999999999996</v>
+        <v>60.125999999999998</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>-893.30399999999997</v>
+        <v>152.46600000000001</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>539.01800000000003</v>
+        <v>671.21500000000003</v>
       </c>
     </row>
     <row r="17" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.35199999999999998</v>
+        <v>0.97599999999999998</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
@@ -1144,7 +1144,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>956.99199999999996</v>
+        <v>176.346</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
@@ -1156,61 +1156,61 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>937.17399999999998</v>
+        <v>-90.051000000000002</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>175.82400000000001</v>
+        <v>-765.46699999999998</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="15"/>
-        <v>-202.47399999999999</v>
+        <v>465.16699999999997</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>-822.59199999999998</v>
+        <v>433.07900000000001</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>-652.63</v>
+        <v>-26.773</v>
       </c>
     </row>
     <row r="18" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97799999999999998</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
@@ -1222,55 +1222,55 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>235.82400000000001</v>
+        <v>763.875</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>-843.37</v>
+        <v>-775.85500000000002</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>-345.77</v>
+        <v>333.26</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="15"/>
-        <v>-368.512</v>
+        <v>-835.99900000000002</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>-677.19</v>
+        <v>95.948999999999998</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
@@ -1282,85 +1282,85 @@
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>424.37599999999998</v>
+        <v>953.79499999999996</v>
       </c>
     </row>
     <row r="19" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.51</v>
+        <v>0.98599999999999999</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>-703.50699999999995</v>
+        <v>-773.89800000000002</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>-863.71100000000001</v>
+        <v>-405.08600000000001</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>718.202</v>
+        <v>862.74400000000003</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="M19">
         <f t="shared" ca="1" si="15"/>
-        <v>914.51199999999994</v>
+        <v>-472.70400000000001</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>-968.83399999999995</v>
+        <v>598.76099999999997</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>945.33</v>
+        <v>198.26499999999999</v>
       </c>
     </row>
     <row r="20" spans="1:25" collapsed="1" x14ac:dyDescent="0.25">
@@ -1443,16 +1443,14 @@
         <f>+A21-D21-G21*J21-M21-P21+S21</f>
         <v>-561591.48616900004</v>
       </c>
-      <c r="W21" s="3">
-        <v>-561591.48616900004</v>
-      </c>
+      <c r="W21" s="3"/>
       <c r="X21" s="1" t="str">
         <f>IF(U21=V21,"match","oops")</f>
         <v>match</v>
       </c>
       <c r="Y21" s="5" t="str">
         <f>IF(W21=V21,"Pass","Fail")</f>
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
     </row>
     <row r="22" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Limit max digits to 14
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="13">
   <si>
     <t>.</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Mine Last Answer</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -106,6 +112,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -119,13 +131,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="W27" sqref="W27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -447,7 +463,7 @@
     <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="12" max="12" width="9.140625" collapsed="1"/>
-    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="15" max="15" width="9.140625" collapsed="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
@@ -456,20 +472,21 @@
     <col min="19" max="19" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.7109375" customWidth="1"/>
     <col min="22" max="23" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-447.34399999999999</v>
+        <v>-838.40200000000004</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="str">
         <f ca="1">VLOOKUP(B1,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -484,15 +501,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>923.54700000000003</v>
+        <v>-483.11200000000002</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -504,15 +521,15 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>-726.47199999999998</v>
+        <v>-858.548</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -524,15 +541,15 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>916.73699999999997</v>
+        <v>-563.00800000000004</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -544,15 +561,15 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-966.07799999999997</v>
+        <v>-364.10700000000003</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -564,7 +581,7 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>154.07400000000001</v>
+        <v>-46.189</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
@@ -578,7 +595,7 @@
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>740.30799999999999</v>
+        <v>949.85900000000004</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -586,19 +603,19 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.85799999999999998</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">VLOOKUP(B10,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>72.694000000000003</v>
+        <v>-775.44200000000001</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -610,7 +627,7 @@
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>162.69399999999999</v>
+        <v>-419.00400000000002</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -622,19 +639,19 @@
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-541.57299999999998</v>
+        <v>-903.69</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L10" t="str">
         <f ca="1">VLOOKUP(K10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
-      </c>
-      <c r="M10">
+        <v>times</v>
+      </c>
+      <c r="M10" s="6">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-993.10299999999995</v>
+        <v>-655.57</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -646,7 +663,7 @@
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>979.8</v>
+        <v>112.958</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -658,73 +675,73 @@
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-982.76700000000005</v>
+        <v>-920.80700000000002</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.94899999999999995</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:C19" ca="1" si="5">VLOOKUP(B11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-898.56100000000004</v>
+        <v>319.83199999999999</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-855.88199999999995</v>
+        <v>-977.79499999999996</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ref="I11:I19" ca="1" si="11">VLOOKUP(H11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>829.45</v>
+        <v>62.420999999999999</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:L19" ca="1" si="14">VLOOKUP(K11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
-      </c>
-      <c r="M11">
+        <v>times</v>
+      </c>
+      <c r="M11" s="6">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>883.173</v>
+        <v>189.01</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O19" ca="1" si="17">VLOOKUP(N11,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>26.739000000000001</v>
+        <v>676.63499999999999</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
@@ -736,127 +753,127 @@
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-389.79</v>
+        <v>55.146999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.73499999999999999</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>-411.267</v>
+        <v>351.51600000000002</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>-123.19799999999999</v>
+        <v>27.962</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>505.47199999999998</v>
+        <v>202.792</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
-      </c>
-      <c r="M12">
+        <v>divide</v>
+      </c>
+      <c r="M12" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>524.79</v>
+        <v>-78.239000000000004</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>-830.83299999999997</v>
+        <v>-581.34100000000001</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>-757.57500000000005</v>
+        <v>-532.69100000000003</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.40500000000000003</v>
+        <v>0.93200000000000005</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>-946.05399999999997</v>
+        <v>120.334</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>-845.68799999999999</v>
+        <v>-933.98299999999995</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>-475.28500000000003</v>
+        <v>35.371000000000002</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
@@ -866,51 +883,51 @@
         <f t="shared" ca="1" si="14"/>
         <v>add</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-524.42499999999995</v>
+        <v>-259.91199999999998</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>-48.222999999999999</v>
+        <v>99.451999999999998</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>-556.00400000000002</v>
+        <v>-962.96799999999996</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67900000000000005</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>962.678</v>
+        <v>-102.96899999999999</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
@@ -922,7 +939,7 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>538.59900000000005</v>
+        <v>-129.38399999999999</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
@@ -934,19 +951,19 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>-61.835999999999999</v>
+        <v>300.80399999999997</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
-      </c>
-      <c r="M14">
+        <v>add</v>
+      </c>
+      <c r="M14" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-184.00399999999999</v>
+        <v>-484.30900000000003</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
@@ -958,49 +975,49 @@
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>-149.11199999999999</v>
+        <v>702.80700000000002</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>808.51499999999999</v>
+        <v>164.54</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.68200000000000005</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>-372.24200000000002</v>
+        <v>-61.21</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>-29.215</v>
+        <v>-968.94500000000005</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
@@ -1012,61 +1029,61 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>-63.451000000000001</v>
+        <v>476.96499999999997</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
-      </c>
-      <c r="M15">
+        <v>times</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-783.36699999999996</v>
+        <v>-806.96199999999999</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>-801.18</v>
+        <v>409.44900000000001</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>-971.82799999999997</v>
+        <v>-92.94</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.72699999999999998</v>
+        <v>0.88100000000000001</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>537.93799999999999</v>
+        <v>3.8679999999999999</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
@@ -1078,7 +1095,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>61.238999999999997</v>
+        <v>141.292</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
@@ -1090,73 +1107,73 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>-968.55</v>
+        <v>-852.67600000000004</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
-      </c>
-      <c r="M16">
+        <v>times</v>
+      </c>
+      <c r="M16" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>60.125999999999998</v>
+        <v>994.48599999999999</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>152.46600000000001</v>
+        <v>-619.15700000000004</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>671.21500000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>-302.94499999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97599999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>176.346</v>
+        <v>-987.09</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>-90.051000000000002</v>
+        <v>502.29500000000002</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
@@ -1168,19 +1185,19 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>-765.46699999999998</v>
+        <v>583.71600000000001</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
-      </c>
-      <c r="M17">
+        <v>minus</v>
+      </c>
+      <c r="M17" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>465.16699999999997</v>
+        <v>83.712000000000003</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
@@ -1192,25 +1209,25 @@
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>433.07900000000001</v>
+        <v>-507.04700000000003</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>-26.773</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>270.971</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.35799999999999998</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
@@ -1222,43 +1239,43 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>763.875</v>
+        <v>221.994</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>-775.85500000000002</v>
+        <v>-707.16600000000005</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>333.26</v>
+        <v>552.35699999999997</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
-      </c>
-      <c r="M18">
+        <v>times</v>
+      </c>
+      <c r="M18" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-835.99900000000002</v>
+        <v>-624.04999999999995</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
@@ -1270,25 +1287,25 @@
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>95.948999999999998</v>
+        <v>-855.24099999999999</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>953.79499999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>-944.93200000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.98599999999999999</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
@@ -1300,70 +1317,70 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>-773.89800000000002</v>
+        <v>-915.77099999999996</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>-405.08600000000001</v>
+        <v>452.75900000000001</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>862.74400000000003</v>
+        <v>640.33600000000001</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
-      </c>
-      <c r="M19">
+        <v>divide</v>
+      </c>
+      <c r="M19" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-472.70400000000001</v>
+        <v>417.15899999999999</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>598.76099999999997</v>
+        <v>935.43799999999999</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>198.26499999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" collapsed="1" x14ac:dyDescent="0.25">
+        <v>-491.36399999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">
       <c r="U20" t="s">
         <v>7</v>
       </c>
@@ -1373,11 +1390,17 @@
       <c r="W20" t="s">
         <v>9</v>
       </c>
-      <c r="Y20" t="s">
+      <c r="X20" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>931.24599999999998</v>
       </c>
@@ -1414,7 +1437,7 @@
       <c r="L21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M21" s="1">
+      <c r="M21" s="7">
         <v>-751.02200000000005</v>
       </c>
       <c r="N21" s="1">
@@ -1443,17 +1466,26 @@
         <f>+A21-D21-G21*J21-M21-P21+S21</f>
         <v>-561591.48616900004</v>
       </c>
-      <c r="W21" s="3"/>
-      <c r="X21" s="1" t="str">
+      <c r="W21" s="3">
+        <v>-561591.48616900004</v>
+      </c>
+      <c r="X21" s="3">
+        <v>-561591.48616900004</v>
+      </c>
+      <c r="Y21" s="1" t="str">
         <f>IF(U21=V21,"match","oops")</f>
         <v>match</v>
       </c>
-      <c r="Y21" s="5" t="str">
+      <c r="Z21" s="5" t="str">
         <f>IF(W21=V21,"Pass","Fail")</f>
-        <v>Fail</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>Pass</v>
+      </c>
+      <c r="AA21" s="5" t="str">
+        <f>IF(X21=W21,"Pass","Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>-678.53</v>
       </c>
@@ -1490,7 +1522,7 @@
       <c r="L22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M22" s="1">
+      <c r="M22" s="7">
         <v>975.65200000000004</v>
       </c>
       <c r="N22" s="1">
@@ -1519,17 +1551,26 @@
         <f>A22*D22+G22+J22+M22-P22*S22</f>
         <v>-759413.141466</v>
       </c>
-      <c r="W22" s="3"/>
-      <c r="X22" s="1" t="str">
+      <c r="W22" s="3">
+        <v>-759413.141466</v>
+      </c>
+      <c r="X22" s="3">
+        <v>-759413.141466</v>
+      </c>
+      <c r="Y22" s="1" t="str">
         <f>IF(U22=V22,"match","oops")</f>
         <v>match</v>
       </c>
-      <c r="Y22" s="5" t="str">
-        <f t="shared" ref="Y22:Y31" si="22">IF(W22=V22,"Pass","Fail")</f>
-        <v>Fail</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Z22" s="5" t="str">
+        <f t="shared" ref="Z22:Z31" si="22">IF(W22=V22,"Pass","Fail")</f>
+        <v>Pass</v>
+      </c>
+      <c r="AA22" s="5" t="str">
+        <f t="shared" ref="AA22:AA31" si="23">IF(X22=W22,"Pass","Fail")</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>-943.84</v>
       </c>
@@ -1548,7 +1589,7 @@
       <c r="F23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="7">
         <v>-555.19100000000003</v>
       </c>
       <c r="H23" s="1">
@@ -1566,7 +1607,7 @@
       <c r="L23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="8">
         <v>-693.20699999999999</v>
       </c>
       <c r="N23" s="1">
@@ -1595,17 +1636,25 @@
         <f>+A23-D23-G23-J23+M23+P23/S23</f>
         <v>-1129.5292548137643</v>
       </c>
-      <c r="W23" s="3"/>
-      <c r="X23" s="1" t="str">
-        <f t="shared" ref="X23:X31" si="23">IF(U23=V23,"match","oops")</f>
+      <c r="W23" s="3">
+        <v>-1129.5292548138</v>
+      </c>
+      <c r="X23" s="3">
+        <v>-1129.5292548138</v>
+      </c>
+      <c r="Y23" s="1" t="str">
+        <f t="shared" ref="Y23:Y31" si="24">IF(U23=V23,"match","oops")</f>
         <v>match</v>
       </c>
-      <c r="Y23" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>Fail</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Z23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA23" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>-782.74300000000005</v>
       </c>
@@ -1633,7 +1682,7 @@
       <c r="I24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="7">
         <v>681.24800000000005</v>
       </c>
       <c r="K24" s="1">
@@ -1642,7 +1691,7 @@
       <c r="L24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M24" s="1">
+      <c r="M24" s="8">
         <v>-278.95699999999999</v>
       </c>
       <c r="N24" s="1">
@@ -1671,17 +1720,26 @@
         <f>+A24*D24-G24*J24/M24*P24*S24</f>
         <v>342557163.22382927</v>
       </c>
-      <c r="W24" s="3"/>
-      <c r="X24" s="1" t="str">
+      <c r="W24" s="3">
+        <v>342557163.22382897</v>
+      </c>
+      <c r="X24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1" t="str">
+        <f t="shared" si="24"/>
+        <v>match</v>
+      </c>
+      <c r="Z24" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>Pass</v>
+      </c>
+      <c r="AA24" s="5" t="str">
         <f t="shared" si="23"/>
-        <v>match</v>
-      </c>
-      <c r="Y24" s="5" t="str">
-        <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
     </row>
-    <row r="25" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>0.59899999999999998</v>
       </c>
@@ -1700,7 +1758,7 @@
       <c r="F25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="7">
         <v>-375.38299999999998</v>
       </c>
       <c r="H25" s="1">
@@ -1718,7 +1776,7 @@
       <c r="L25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M25" s="1">
+      <c r="M25" s="8">
         <v>-166.291</v>
       </c>
       <c r="N25" s="1">
@@ -1748,16 +1806,23 @@
         <v>150910.71995797154</v>
       </c>
       <c r="W25" s="3"/>
-      <c r="X25" s="1" t="str">
-        <f t="shared" si="23"/>
+      <c r="X25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="1" t="str">
+        <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Y25" s="5" t="str">
+      <c r="Z25" s="5" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA25" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>333.08</v>
       </c>
@@ -1794,7 +1859,7 @@
       <c r="L26" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M26" s="1">
+      <c r="M26" s="8">
         <v>-0.159</v>
       </c>
       <c r="N26" s="1">
@@ -1803,7 +1868,7 @@
       <c r="O26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P26" s="1">
+      <c r="P26" s="7">
         <v>245.52699999999999</v>
       </c>
       <c r="Q26" s="1">
@@ -1824,16 +1889,23 @@
         <v>150.30844325911923</v>
       </c>
       <c r="W26" s="3"/>
-      <c r="X26" s="1" t="str">
-        <f t="shared" si="23"/>
+      <c r="X26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="1" t="str">
+        <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Y26" s="5" t="str">
+      <c r="Z26" s="5" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA26" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>-602.952</v>
       </c>
@@ -1870,7 +1942,7 @@
       <c r="L27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M27" s="1">
+      <c r="M27" s="7">
         <v>-313.05900000000003</v>
       </c>
       <c r="N27" s="1">
@@ -1900,16 +1972,23 @@
         <v>-551042.36246835184</v>
       </c>
       <c r="W27" s="3"/>
-      <c r="X27" s="1" t="str">
-        <f t="shared" si="23"/>
+      <c r="X27" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="1" t="str">
+        <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Y27" s="5" t="str">
+      <c r="Z27" s="5" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA27" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>391.702</v>
       </c>
@@ -1946,7 +2025,7 @@
       <c r="L28" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M28" s="1">
+      <c r="M28" s="8">
         <v>-533.02099999999996</v>
       </c>
       <c r="N28" s="1">
@@ -1964,7 +2043,7 @@
       <c r="R28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S28" s="1">
+      <c r="S28" s="7">
         <v>-948.32799999999997</v>
       </c>
       <c r="U28" s="2">
@@ -1976,16 +2055,23 @@
         <v>-292421.6855380105</v>
       </c>
       <c r="W28" s="3"/>
-      <c r="X28" s="1" t="str">
-        <f t="shared" si="23"/>
+      <c r="X28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="1" t="str">
+        <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Y28" s="5" t="str">
+      <c r="Z28" s="5" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA28" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>429.351</v>
       </c>
@@ -2022,7 +2108,7 @@
       <c r="L29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="M29" s="1">
+      <c r="M29" s="8">
         <v>-463.44099999999997</v>
       </c>
       <c r="N29" s="1">
@@ -2031,7 +2117,7 @@
       <c r="O29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P29" s="1">
+      <c r="P29" s="7">
         <v>-0.26300000000000001</v>
       </c>
       <c r="Q29" s="1">
@@ -2052,16 +2138,23 @@
         <v>-94248115.529089928</v>
       </c>
       <c r="W29" s="3"/>
-      <c r="X29" s="1" t="str">
-        <f t="shared" si="23"/>
+      <c r="X29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="1" t="str">
+        <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Y29" s="5" t="str">
+      <c r="Z29" s="5" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA29" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>320.38900000000001</v>
       </c>
@@ -2098,7 +2191,7 @@
       <c r="L30" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="M30" s="1">
+      <c r="M30" s="7">
         <v>627.71100000000001</v>
       </c>
       <c r="N30" s="1">
@@ -2128,16 +2221,23 @@
         <v>156881.74130299999</v>
       </c>
       <c r="W30" s="3"/>
-      <c r="X30" s="1" t="str">
-        <f t="shared" si="23"/>
+      <c r="X30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="1" t="str">
+        <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Y30" s="5" t="str">
+      <c r="Z30" s="5" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="AA30" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>931.24599999999998</v>
       </c>
@@ -2156,13 +2256,13 @@
       <c r="I31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="1">
+      <c r="J31" s="7">
         <v>681.24800000000005</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M31" s="1">
+      <c r="M31" s="8">
         <v>-0.159</v>
       </c>
       <c r="O31" s="1" t="s">
@@ -2186,14 +2286,42 @@
         <v>1647247726.4280634</v>
       </c>
       <c r="W31" s="4"/>
-      <c r="X31" s="1" t="str">
-        <f t="shared" si="23"/>
+      <c r="X31" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="1" t="str">
+        <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Y31" s="5" t="str">
+      <c r="Z31" s="5" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
+      <c r="AA31" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="M32" s="9"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M33" s="9"/>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M34" s="9"/>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M35" s="9"/>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M36" s="9"/>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M37" s="9"/>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M38" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limit decimal places to 10
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="13">
   <si>
     <t>.</t>
   </si>
@@ -93,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +118,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -131,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -142,6 +148,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,7 +454,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -478,15 +486,15 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-838.40200000000004</v>
+        <v>-79.793999999999997</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C1" t="str">
         <f ca="1">VLOOKUP(B1,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -501,15 +509,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-483.11200000000002</v>
+        <v>433.64</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -521,15 +529,15 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>-858.548</v>
+        <v>-226.53899999999999</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -541,7 +549,7 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>-563.00800000000004</v>
+        <v>573.63599999999997</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
@@ -561,15 +569,15 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-364.10700000000003</v>
+        <v>963.05600000000004</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -581,7 +589,7 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>-46.189</v>
+        <v>656.28899999999999</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
@@ -595,7 +603,7 @@
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>949.85900000000004</v>
+        <v>870.44200000000001</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -603,43 +611,43 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.16200000000000001</v>
+        <v>0.153</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">VLOOKUP(B10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-775.44200000000001</v>
+        <v>839.13499999999999</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(E10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-419.00400000000002</v>
+        <v>-589.03499999999997</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-903.69</v>
+        <v>-304.161</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -651,19 +659,19 @@
       </c>
       <c r="M10" s="6">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-655.57</v>
+        <v>69.05</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O10" t="str">
         <f ca="1">VLOOKUP(N10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>112.958</v>
+        <v>-77.728999999999999</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -675,13 +683,13 @@
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-920.80700000000002</v>
+        <v>-873.33399999999995</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.34300000000000003</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
@@ -693,43 +701,43 @@
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>319.83199999999999</v>
+        <v>164.65600000000001</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-977.79499999999996</v>
+        <v>-660.36800000000005</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ref="I11:I19" ca="1" si="11">VLOOKUP(H11,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>62.420999999999999</v>
+        <v>815.25199999999995</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:L19" ca="1" si="14">VLOOKUP(K11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>189.01</v>
+        <v>412.44400000000002</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
@@ -741,25 +749,25 @@
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>676.63499999999999</v>
+        <v>435.48700000000002</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ref="R11:R19" ca="1" si="20">VLOOKUP(Q11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>55.146999999999998</v>
+        <v>95.525000000000006</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.59399999999999997</v>
+        <v>0.51900000000000002</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
@@ -771,7 +779,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>351.51600000000002</v>
+        <v>757.74300000000005</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
@@ -783,61 +791,61 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>27.962</v>
+        <v>-23.38</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>202.792</v>
+        <v>-626.67499999999995</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-78.239000000000004</v>
+        <v>-979.80899999999997</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>-581.34100000000001</v>
+        <v>-620.54899999999998</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>-532.69100000000003</v>
+        <v>578.48400000000004</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.93200000000000005</v>
+        <v>0.99299999999999999</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
@@ -849,121 +857,121 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>120.334</v>
+        <v>-54.366999999999997</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>-933.98299999999995</v>
+        <v>-350.18700000000001</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>35.371000000000002</v>
+        <v>118.59099999999999</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="M13" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-259.91199999999998</v>
+        <v>47.05</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>99.451999999999998</v>
+        <v>112.904</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>-962.96799999999996</v>
+        <v>582.50300000000004</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.47599999999999998</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>-102.96899999999999</v>
+        <v>-634.75</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>-129.38399999999999</v>
+        <v>-924.11500000000001</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>300.80399999999997</v>
+        <v>552.87099999999998</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-484.30900000000003</v>
+        <v>-488.50900000000001</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
@@ -975,25 +983,25 @@
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>702.80700000000002</v>
+        <v>-548.15099999999995</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>164.54</v>
+        <v>279.60300000000001</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>5.0000000000000001E-3</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
@@ -1005,151 +1013,151 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>-61.21</v>
+        <v>-724.22299999999996</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>-968.94500000000005</v>
+        <v>-338.18700000000001</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>476.96499999999997</v>
+        <v>266.61700000000002</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-806.96199999999999</v>
+        <v>521.48</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>409.44900000000001</v>
+        <v>304.572</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>-92.94</v>
+        <v>-498.95800000000003</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.88100000000000001</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>3.8679999999999999</v>
+        <v>-553.51599999999996</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>141.292</v>
+        <v>779.94799999999998</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>-852.67600000000004</v>
+        <v>914.85299999999995</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>994.48599999999999</v>
+        <v>762.90300000000002</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>-619.15700000000004</v>
+        <v>723.70899999999995</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>-302.94499999999999</v>
+        <v>-152.583</v>
       </c>
     </row>
     <row r="17" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.19</v>
+        <v>0.97</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
@@ -1161,7 +1169,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>-987.09</v>
+        <v>924.66499999999996</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
@@ -1173,19 +1181,19 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>502.29500000000002</v>
+        <v>-411.17899999999997</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>583.71600000000001</v>
+        <v>-509.56099999999998</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
@@ -1197,19 +1205,19 @@
       </c>
       <c r="M17" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>83.712000000000003</v>
+        <v>-521.53099999999995</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>-507.04700000000003</v>
+        <v>354.41399999999999</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
@@ -1221,37 +1229,37 @@
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>270.971</v>
+        <v>155.804</v>
       </c>
     </row>
     <row r="18" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97699999999999998</v>
+        <v>0.218</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>221.994</v>
+        <v>-934.24599999999998</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>-707.16600000000005</v>
+        <v>-117.18</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
@@ -1263,49 +1271,49 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>552.35699999999997</v>
+        <v>-594.25599999999997</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-624.04999999999995</v>
+        <v>107.85599999999999</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>-855.24099999999999</v>
+        <v>-393.55799999999999</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>-944.93200000000002</v>
+        <v>-445.11</v>
       </c>
     </row>
     <row r="19" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.34499999999999997</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
@@ -1317,7 +1325,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>-915.77099999999996</v>
+        <v>421.209</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
@@ -1329,7 +1337,7 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>452.75900000000001</v>
+        <v>-995.48699999999997</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
@@ -1341,19 +1349,19 @@
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>640.33600000000001</v>
+        <v>-936.18</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>417.15899999999999</v>
+        <v>334.411</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
@@ -1365,7 +1373,7 @@
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>935.43799999999999</v>
+        <v>-450.73</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
@@ -1377,7 +1385,7 @@
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>-491.36399999999998</v>
+        <v>358.32900000000001</v>
       </c>
     </row>
     <row r="20" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">
@@ -1654,89 +1662,88 @@
         <v>Pass</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
+    <row r="24" spans="1:27" s="10" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
         <v>-782.74300000000005</v>
       </c>
-      <c r="B24" s="1">
-        <v>3</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="B24" s="10">
+        <v>3</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="10">
         <v>-642.74099999999999</v>
       </c>
-      <c r="E24" s="1">
-        <v>2</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G24" s="1">
+      <c r="E24" s="10">
+        <v>2</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="10">
         <v>517.48900000000003</v>
       </c>
-      <c r="H24" s="1">
-        <v>3</v>
-      </c>
-      <c r="I24" s="1" t="s">
+      <c r="H24" s="10">
+        <v>3</v>
+      </c>
+      <c r="I24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J24" s="7">
+      <c r="J24" s="10">
         <v>681.24800000000005</v>
       </c>
-      <c r="K24" s="1">
-        <v>4</v>
-      </c>
-      <c r="L24" s="1" t="s">
+      <c r="K24" s="10">
+        <v>4</v>
+      </c>
+      <c r="L24" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="M24" s="8">
+      <c r="M24" s="10">
         <v>-278.95699999999999</v>
       </c>
-      <c r="N24" s="1">
-        <v>3</v>
-      </c>
-      <c r="O24" s="1" t="s">
+      <c r="N24" s="10">
+        <v>3</v>
+      </c>
+      <c r="O24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="P24" s="1">
+      <c r="P24" s="10">
         <v>712.05399999999997</v>
       </c>
-      <c r="Q24" s="1">
-        <v>3</v>
-      </c>
-      <c r="R24" s="1" t="s">
+      <c r="Q24" s="10">
+        <v>3</v>
+      </c>
+      <c r="R24" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="S24" s="1">
+      <c r="S24" s="10">
         <v>380.113</v>
       </c>
-      <c r="U24" s="2">
+      <c r="U24" s="11">
         <f>+A24*D24-G24*J24/M24*P24*S24</f>
         <v>342557163.22382927</v>
       </c>
-      <c r="V24" s="2">
+      <c r="V24" s="11">
         <f>+A24*D24-G24*J24/M24*P24*S24</f>
         <v>342557163.22382927</v>
       </c>
-      <c r="W24" s="3">
+      <c r="W24" s="11">
         <v>342557163.22382897</v>
       </c>
-      <c r="X24" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="1" t="str">
+      <c r="X24" s="11">
+        <v>342557163.22382998</v>
+      </c>
+      <c r="Y24" s="10" t="str">
         <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Z24" s="5" t="str">
+      <c r="Z24" s="11" t="str">
         <f t="shared" si="22"/>
         <v>Pass</v>
       </c>
-      <c r="AA24" s="5" t="str">
-        <f t="shared" si="23"/>
-        <v>Fail</v>
+      <c r="AA24" s="11" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1805,7 +1812,9 @@
         <f>+A25/D25-G25-J25-M25*P25+S25</f>
         <v>150910.71995797154</v>
       </c>
-      <c r="W25" s="3"/>
+      <c r="W25" s="3">
+        <v>150910.71995797</v>
+      </c>
       <c r="X25" s="3">
         <v>0</v>
       </c>
@@ -1813,13 +1822,12 @@
         <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Z25" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>Fail</v>
+      <c r="Z25" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="AA25" s="5" t="str">
         <f t="shared" si="23"/>
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
     </row>
     <row r="26" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update readme. Rename to Calculator
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
   <si>
     <t>.</t>
   </si>
@@ -137,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -150,6 +150,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +458,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -473,7 +477,7 @@
     <col min="12" max="12" width="9.140625" collapsed="1"/>
     <col min="13" max="13" width="12.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="9.140625" collapsed="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="0" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="18" max="18" width="9.140625" collapsed="1"/>
@@ -486,15 +490,15 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-79.793999999999997</v>
+        <v>533.84400000000005</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" t="str">
         <f ca="1">VLOOKUP(B1,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -509,15 +513,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>433.64</v>
+        <v>943.755</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -529,7 +533,7 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>-226.53899999999999</v>
+        <v>955.93799999999999</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
@@ -549,15 +553,15 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>573.63599999999997</v>
+        <v>496.44600000000003</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -569,7 +573,7 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>963.05600000000004</v>
+        <v>-501.01299999999998</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
@@ -589,21 +593,21 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>656.28899999999999</v>
+        <v>777.91800000000001</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
     </row>
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>870.44200000000001</v>
+        <v>-712.28899999999999</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -611,7 +615,7 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.153</v>
+        <v>0.53400000000000003</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -623,73 +627,73 @@
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>839.13499999999999</v>
+        <v>-69.129000000000005</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(E10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-589.03499999999997</v>
+        <v>-811.548</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-304.161</v>
+        <v>-180.47399999999999</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L10" t="str">
         <f ca="1">VLOOKUP(K10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="M10" s="6">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>69.05</v>
+        <v>193.339</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O10" t="str">
         <f ca="1">VLOOKUP(N10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-77.728999999999999</v>
+        <v>585.51</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R10" t="str">
         <f ca="1">VLOOKUP(Q10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-873.33399999999995</v>
+        <v>64.212000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.16400000000000001</v>
+        <v>0.71799999999999997</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
@@ -701,31 +705,31 @@
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>164.65600000000001</v>
+        <v>250.405</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-660.36800000000005</v>
+        <v>-278.99700000000001</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ref="I11:I19" ca="1" si="11">VLOOKUP(H11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>815.25199999999995</v>
+        <v>393.738</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
@@ -737,7 +741,7 @@
       </c>
       <c r="M11" s="6">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>412.44400000000002</v>
+        <v>-203.39599999999999</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
@@ -749,127 +753,127 @@
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>435.48700000000002</v>
+        <v>306.26600000000002</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ref="R11:R19" ca="1" si="20">VLOOKUP(Q11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>95.525000000000006</v>
+        <v>-146.12799999999999</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.51900000000000002</v>
+        <v>0.95699999999999996</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>757.74300000000005</v>
+        <v>911.14800000000002</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>-23.38</v>
+        <v>269.62</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>-626.67499999999995</v>
+        <v>-828.23599999999999</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-979.80899999999997</v>
+        <v>-668.59900000000005</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>-620.54899999999998</v>
+        <v>-821.2</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>578.48400000000004</v>
+        <v>85.26</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.99299999999999999</v>
+        <v>0.82699999999999996</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>-54.366999999999997</v>
+        <v>-412.05099999999999</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>-350.18700000000001</v>
+        <v>-54.137999999999998</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
@@ -881,7 +885,7 @@
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>118.59099999999999</v>
+        <v>999.99800000000005</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
@@ -893,97 +897,97 @@
       </c>
       <c r="M13" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>47.05</v>
+        <v>10.648</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>112.904</v>
+        <v>-836.56200000000001</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>582.50300000000004</v>
+        <v>-998.55100000000004</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.76300000000000001</v>
+        <v>0.58899999999999997</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>-634.75</v>
+        <v>-974.91200000000003</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>-924.11500000000001</v>
+        <v>-238.459</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>552.87099999999998</v>
+        <v>420.49599999999998</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-488.50900000000001</v>
+        <v>-804.904</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>-548.15099999999995</v>
+        <v>-436.15699999999998</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
@@ -995,61 +999,61 @@
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>279.60300000000001</v>
+        <v>-588.61099999999999</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.16200000000000001</v>
+        <v>0.57799999999999996</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>-724.22299999999996</v>
+        <v>-50.491999999999997</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>-338.18700000000001</v>
+        <v>820.20699999999999</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>266.61700000000002</v>
+        <v>-298.99799999999999</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>521.48</v>
+        <v>137.309</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
@@ -1061,73 +1065,73 @@
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>304.572</v>
+        <v>720.18799999999999</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>-498.95800000000003</v>
+        <v>265.58</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>7.0999999999999994E-2</v>
+        <v>0.61299999999999999</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>-553.51599999999996</v>
+        <v>99.316000000000003</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>779.94799999999998</v>
+        <v>563.29200000000003</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>914.85299999999995</v>
+        <v>521.173</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>762.90300000000002</v>
+        <v>385.80099999999999</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
@@ -1139,127 +1143,127 @@
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>723.70899999999995</v>
+        <v>504.76400000000001</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>-152.583</v>
+        <v>497.18</v>
       </c>
     </row>
     <row r="17" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97</v>
+        <v>0.90600000000000003</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>924.66499999999996</v>
+        <v>-297.10500000000002</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>-411.17899999999997</v>
+        <v>380.005</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>-509.56099999999998</v>
+        <v>-131.733</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-521.53099999999995</v>
+        <v>-72.262</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>354.41399999999999</v>
+        <v>723.10400000000004</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>155.804</v>
+        <v>150.53100000000001</v>
       </c>
     </row>
     <row r="18" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.218</v>
+        <v>0.52800000000000002</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>-934.24599999999998</v>
+        <v>920.46100000000001</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>-117.18</v>
+        <v>-588.89200000000005</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
@@ -1271,19 +1275,19 @@
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>-594.25599999999997</v>
+        <v>-524.346</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>107.85599999999999</v>
+        <v>880.11</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
@@ -1295,7 +1299,7 @@
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>-393.55799999999999</v>
+        <v>-359.10700000000003</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
@@ -1307,61 +1311,61 @@
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>-445.11</v>
+        <v>-199.74100000000001</v>
       </c>
     </row>
     <row r="19" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.36399999999999999</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>421.209</v>
+        <v>759.11300000000006</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>-995.48699999999997</v>
+        <v>-898.98099999999999</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>-936.18</v>
+        <v>347.16199999999998</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>334.411</v>
+        <v>997.88800000000003</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
@@ -1373,7 +1377,7 @@
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>-450.73</v>
+        <v>-680.93600000000004</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
@@ -1385,7 +1389,7 @@
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>358.32900000000001</v>
+        <v>389.62400000000002</v>
       </c>
     </row>
     <row r="20" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">
@@ -1816,7 +1820,7 @@
         <v>150910.71995797</v>
       </c>
       <c r="X25" s="3">
-        <v>0</v>
+        <v>150910.71995797</v>
       </c>
       <c r="Y25" s="1" t="str">
         <f t="shared" si="24"/>
@@ -1827,7 +1831,7 @@
       </c>
       <c r="AA25" s="5" t="str">
         <f t="shared" si="23"/>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
     </row>
     <row r="26" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1896,102 +1900,103 @@
         <f>+A26/D26*G26/J26-M26/P26+S26</f>
         <v>150.30844325911923</v>
       </c>
-      <c r="W26" s="3"/>
+      <c r="W26" s="3">
+        <v>150.30844325964</v>
+      </c>
       <c r="X26" s="3">
-        <v>0</v>
+        <v>150.30844325964</v>
       </c>
       <c r="Y26" s="1" t="str">
         <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Z26" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>Fail</v>
+      <c r="Z26" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="AA26" s="5" t="str">
         <f t="shared" si="23"/>
         <v>Pass</v>
       </c>
     </row>
-    <row r="27" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
+    <row r="27" spans="1:27" s="10" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10">
         <v>-602.952</v>
       </c>
-      <c r="B27" s="1">
-        <v>4</v>
-      </c>
-      <c r="C27" s="1" t="s">
+      <c r="B27" s="10">
+        <v>4</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="10">
         <v>387.71800000000002</v>
       </c>
-      <c r="E27" s="1">
-        <v>4</v>
-      </c>
-      <c r="F27" s="1" t="s">
+      <c r="E27" s="10">
+        <v>4</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="10">
         <v>849.43899999999996</v>
       </c>
-      <c r="H27" s="1">
-        <v>3</v>
-      </c>
-      <c r="I27" s="1" t="s">
+      <c r="H27" s="10">
+        <v>3</v>
+      </c>
+      <c r="I27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J27" s="10">
         <v>903.17499999999995</v>
       </c>
-      <c r="K27" s="1">
-        <v>3</v>
-      </c>
-      <c r="L27" s="1" t="s">
+      <c r="K27" s="10">
+        <v>3</v>
+      </c>
+      <c r="L27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="10">
         <v>-313.05900000000003</v>
       </c>
-      <c r="N27" s="1">
-        <v>1</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P27" s="1">
+      <c r="N27" s="10">
+        <v>1</v>
+      </c>
+      <c r="O27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="P27" s="7">
         <v>695.24400000000003</v>
       </c>
-      <c r="Q27" s="1">
-        <v>3</v>
-      </c>
-      <c r="R27" s="1" t="s">
+      <c r="Q27" s="10">
+        <v>3</v>
+      </c>
+      <c r="R27" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="S27" s="1">
+      <c r="S27" s="10">
         <v>-793.33299999999997</v>
       </c>
-      <c r="U27" s="2">
+      <c r="U27" s="11">
         <f>+A27/D27/G27*J27*M27+P27*S27</f>
         <v>-551042.36246835184</v>
       </c>
-      <c r="V27" s="2">
+      <c r="V27" s="11">
         <f>+A27/D27/G27*J27*M27+P27*S27</f>
         <v>-551042.36246835184</v>
       </c>
-      <c r="W27" s="3"/>
-      <c r="X27" s="3">
+      <c r="W27" s="11"/>
+      <c r="X27" s="11">
         <v>0</v>
       </c>
-      <c r="Y27" s="1" t="str">
+      <c r="Y27" s="10" t="str">
         <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Z27" s="5" t="str">
+      <c r="Z27" s="11" t="str">
         <f t="shared" si="22"/>
         <v>Fail</v>
       </c>
-      <c r="AA27" s="5" t="str">
+      <c r="AA27" s="11" t="str">
         <f t="shared" si="23"/>
         <v>Pass</v>
       </c>
@@ -2062,9 +2067,11 @@
         <f>+A28+D28+G28+J28/M28-P28*S28</f>
         <v>-292421.6855380105</v>
       </c>
-      <c r="W28" s="3"/>
+      <c r="W28" s="3">
+        <v>-292421.68553800997</v>
+      </c>
       <c r="X28" s="3">
-        <v>0</v>
+        <v>-292421.68553800997</v>
       </c>
       <c r="Y28" s="1" t="str">
         <f t="shared" si="24"/>
@@ -2072,7 +2079,7 @@
       </c>
       <c r="Z28" s="5" t="str">
         <f t="shared" si="22"/>
-        <v>Fail</v>
+        <v>Pass</v>
       </c>
       <c r="AA28" s="5" t="str">
         <f t="shared" si="23"/>
@@ -2145,138 +2152,146 @@
         <f>+A29*D29*G29-J29*M29*P29*S29</f>
         <v>-94248115.529089928</v>
       </c>
-      <c r="W29" s="3"/>
+      <c r="W29" s="3">
+        <v>-94248115.529090002</v>
+      </c>
       <c r="X29" s="3">
-        <v>0</v>
+        <v>-94248115.529090002</v>
       </c>
       <c r="Y29" s="1" t="str">
         <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Z29" s="5" t="str">
-        <f t="shared" si="22"/>
-        <v>Fail</v>
+      <c r="Z29" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="AA29" s="5" t="str">
         <f t="shared" si="23"/>
         <v>Pass</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
+    <row r="30" spans="1:27" s="10" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10">
         <v>320.38900000000001</v>
       </c>
-      <c r="B30" s="1">
-        <v>3</v>
-      </c>
-      <c r="C30" s="1" t="s">
+      <c r="B30" s="10">
+        <v>3</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="10">
         <v>490.22699999999998</v>
       </c>
-      <c r="E30" s="1">
-        <v>2</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G30" s="1">
+      <c r="E30" s="10">
+        <v>2</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="10">
         <v>0.34200000000000003</v>
       </c>
-      <c r="H30" s="1">
-        <v>1</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" s="1">
+      <c r="H30" s="10">
+        <v>1</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="10">
         <v>966.53800000000001</v>
       </c>
-      <c r="K30" s="1">
-        <v>2</v>
-      </c>
-      <c r="L30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M30" s="7">
+      <c r="K30" s="10">
+        <v>2</v>
+      </c>
+      <c r="L30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="M30" s="10">
         <v>627.71100000000001</v>
       </c>
-      <c r="N30" s="1">
-        <v>2</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P30" s="1">
+      <c r="N30" s="10">
+        <v>2</v>
+      </c>
+      <c r="O30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P30" s="10">
         <v>-183.1</v>
       </c>
-      <c r="Q30" s="1">
-        <v>2</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="S30" s="1">
+      <c r="Q30" s="10">
+        <v>2</v>
+      </c>
+      <c r="R30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="S30" s="10">
         <v>703.18200000000002</v>
       </c>
-      <c r="U30" s="2">
+      <c r="U30" s="11">
         <f>+A30*D30-G30+J30-M30-P30-S30</f>
         <v>156881.74130299999</v>
       </c>
-      <c r="V30" s="2">
+      <c r="V30" s="11">
         <f>+A30*D30-G30+J30-M30-P30-S30</f>
         <v>156881.74130299999</v>
       </c>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y30" s="1" t="str">
+      <c r="W30" s="11">
+        <v>156881.74130299999</v>
+      </c>
+      <c r="X30" s="11">
+        <v>156881.74130299999</v>
+      </c>
+      <c r="Y30" s="10" t="str">
         <f t="shared" si="24"/>
         <v>match</v>
       </c>
-      <c r="Z30" s="5" t="str">
+      <c r="Z30" s="11" t="str">
         <f t="shared" si="22"/>
-        <v>Fail</v>
-      </c>
-      <c r="AA30" s="5" t="str">
+        <v>Pass</v>
+      </c>
+      <c r="AA30" s="11" t="str">
         <f t="shared" si="23"/>
         <v>Pass</v>
       </c>
     </row>
     <row r="31" spans="1:27" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
+      <c r="A31" s="14">
         <v>931.24599999999998</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="15"/>
+      <c r="C31" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="14">
         <v>934.96100000000001</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="E31" s="13"/>
+      <c r="F31" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="12">
         <v>-555.19100000000003</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="H31" s="13"/>
+      <c r="I31" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="12">
         <v>681.24800000000005</v>
       </c>
-      <c r="L31" s="1" t="s">
+      <c r="K31" s="13"/>
+      <c r="L31" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M31" s="8">
+      <c r="M31" s="12">
         <v>-0.159</v>
       </c>
-      <c r="O31" s="1" t="s">
+      <c r="N31" s="13"/>
+      <c r="O31" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="P31" s="1">
+      <c r="P31" s="12">
         <v>695.24400000000003</v>
       </c>
       <c r="R31" s="1" t="s">
@@ -2293,7 +2308,9 @@
         <f>+A31/D31*G31*J31/M31*P31-S31</f>
         <v>1647247726.4280634</v>
       </c>
-      <c r="W31" s="4"/>
+      <c r="W31" s="3">
+        <v>1647247681.1802001</v>
+      </c>
       <c r="X31" s="4">
         <v>0</v>
       </c>
@@ -2307,28 +2324,51 @@
       </c>
       <c r="AA31" s="5" t="str">
         <f t="shared" si="23"/>
-        <v>Pass</v>
+        <v>Fail</v>
       </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:22" x14ac:dyDescent="0.25">
       <c r="M33" s="9"/>
-    </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <f>931.246/934.961*-555.191*681.248/-0.159*695.244+793.333</f>
+        <v>1647247726.4280634</v>
+      </c>
+      <c r="V33">
+        <v>1647247681.1802001</v>
+      </c>
+    </row>
+    <row r="34" spans="4:22" x14ac:dyDescent="0.25">
       <c r="M34" s="9"/>
     </row>
-    <row r="35" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:22" x14ac:dyDescent="0.25">
       <c r="M35" s="9"/>
-    </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <f>931.246/934.961*-555.191*681.248/-0.159*695.244+793.333</f>
+        <v>1647247726.4280634</v>
+      </c>
+    </row>
+    <row r="36" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <f>931.246/934.961*-555.191*681.248/-0.159*695.244</f>
+        <v>1647246933.0950634</v>
+      </c>
       <c r="M36" s="9"/>
     </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:22" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <f>931.246/934.961</f>
+        <v>0.99602657223135505</v>
+      </c>
+      <c r="I37">
+        <f>1/931.264</f>
+        <v>1.0738093601814309E-3</v>
+      </c>
       <c r="M37" s="9"/>
     </row>
-    <row r="38" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:22" x14ac:dyDescent="0.25">
       <c r="M38" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepend `0` if decimal is first user input
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -490,15 +490,15 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>533.84400000000005</v>
+        <v>-792.33100000000002</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C1" t="str">
         <f ca="1">VLOOKUP(B1,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -513,15 +513,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>943.755</v>
+        <v>48.847999999999999</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -533,7 +533,7 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>955.93799999999999</v>
+        <v>-948.92700000000002</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
@@ -553,15 +553,15 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>496.44600000000003</v>
+        <v>946.97400000000005</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -573,7 +573,7 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-501.01299999999998</v>
+        <v>-536.70699999999999</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
@@ -593,21 +593,21 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>777.91800000000001</v>
+        <v>-774.13800000000003</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>add</v>
+        <v>times</v>
       </c>
     </row>
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>-712.28899999999999</v>
+        <v>-8.2840000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -615,7 +615,7 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.53400000000000003</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -627,55 +627,55 @@
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-69.129000000000005</v>
+        <v>897.923</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(E10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-811.548</v>
+        <v>-979.32299999999998</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-180.47399999999999</v>
+        <v>498.55500000000001</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L10" t="str">
         <f ca="1">VLOOKUP(K10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="M10" s="6">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>193.339</v>
+        <v>-686.28700000000003</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10" t="str">
         <f ca="1">VLOOKUP(N10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>585.51</v>
+        <v>263.97399999999999</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -687,115 +687,115 @@
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>64.212000000000003</v>
+        <v>163.54</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.71799999999999997</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:C19" ca="1" si="5">VLOOKUP(B11,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>250.405</v>
+        <v>592.29399999999998</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-278.99700000000001</v>
+        <v>-851.779</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ref="I11:I19" ca="1" si="11">VLOOKUP(H11,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>393.738</v>
+        <v>-847.49599999999998</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:L19" ca="1" si="14">VLOOKUP(K11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-203.39599999999999</v>
+        <v>-683.57899999999995</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O19" ca="1" si="17">VLOOKUP(N11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>306.26600000000002</v>
+        <v>-928.35900000000004</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ref="R11:R19" ca="1" si="20">VLOOKUP(Q11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-146.12799999999999</v>
+        <v>-770.98400000000004</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.95699999999999996</v>
+        <v>0.68400000000000005</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>911.14800000000002</v>
+        <v>-451.35300000000001</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>269.62</v>
+        <v>-534.45100000000002</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
@@ -807,61 +807,61 @@
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>-828.23599999999999</v>
+        <v>903.53800000000001</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-668.59900000000005</v>
+        <v>734.50699999999995</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>-821.2</v>
+        <v>686.52099999999996</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>85.26</v>
+        <v>-721.79399999999998</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.82699999999999996</v>
+        <v>0.78900000000000003</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>-412.05099999999999</v>
+        <v>449.99200000000002</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
@@ -873,109 +873,109 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>-54.137999999999998</v>
+        <v>-593.04999999999995</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>999.99800000000005</v>
+        <v>923.70799999999997</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="M13" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>10.648</v>
+        <v>-459.57299999999998</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>-836.56200000000001</v>
+        <v>-978.31899999999996</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>-998.55100000000004</v>
+        <v>192.35400000000001</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.58899999999999997</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>-974.91200000000003</v>
+        <v>-133.678</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>-238.459</v>
+        <v>-560.76599999999996</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>420.49599999999998</v>
+        <v>710.50800000000004</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-804.904</v>
+        <v>-466.73399999999998</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
@@ -987,37 +987,37 @@
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>-436.15699999999998</v>
+        <v>233.59200000000001</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>-588.61099999999999</v>
+        <v>-649.63199999999995</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.57799999999999996</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>-50.491999999999997</v>
+        <v>899.02200000000005</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
@@ -1029,43 +1029,43 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>820.20699999999999</v>
+        <v>-808.42399999999998</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>-298.99799999999999</v>
+        <v>-12.257</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>137.309</v>
+        <v>685.63099999999997</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>720.18799999999999</v>
+        <v>222.697</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
@@ -1077,61 +1077,61 @@
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>265.58</v>
+        <v>-888.00300000000004</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.61299999999999999</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>99.316000000000003</v>
+        <v>-827.53300000000002</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>563.29200000000003</v>
+        <v>-329.82400000000001</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>521.173</v>
+        <v>309.995</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>385.80099999999999</v>
+        <v>-939.12300000000005</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>504.76400000000001</v>
+        <v>938.55200000000002</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
@@ -1155,13 +1155,13 @@
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>497.18</v>
+        <v>-535.93100000000004</v>
       </c>
     </row>
     <row r="17" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.90600000000000003</v>
+        <v>0.38</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
@@ -1173,19 +1173,19 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>-297.10500000000002</v>
+        <v>444.41399999999999</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>380.005</v>
+        <v>373.029</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>-131.733</v>
+        <v>-220.96299999999999</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
@@ -1209,127 +1209,127 @@
       </c>
       <c r="M17" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-72.262</v>
+        <v>649.36500000000001</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>723.10400000000004</v>
+        <v>-180.09200000000001</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>150.53100000000001</v>
+        <v>-562.07500000000005</v>
       </c>
     </row>
     <row r="18" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.52800000000000002</v>
+        <v>0.75600000000000001</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>920.46100000000001</v>
+        <v>-770.01499999999999</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>-588.89200000000005</v>
+        <v>-276.62799999999999</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>-524.346</v>
+        <v>953.42600000000004</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>880.11</v>
+        <v>486.91199999999998</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>-359.10700000000003</v>
+        <v>-105.758</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>-199.74100000000001</v>
+        <v>-700.99900000000002</v>
       </c>
     </row>
     <row r="19" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.73099999999999998</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>759.11300000000006</v>
+        <v>274.30099999999999</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
@@ -1341,55 +1341,55 @@
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>-898.98099999999999</v>
+        <v>-477.315</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>347.16199999999998</v>
+        <v>127.00700000000001</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>997.88800000000003</v>
+        <v>605.02800000000002</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>-680.93600000000004</v>
+        <v>897.23099999999999</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>389.62400000000002</v>
+        <v>357.23</v>
       </c>
     </row>
     <row r="20" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add control for preventing redundant starting zeros
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD23"/>
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -490,7 +490,7 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-792.33100000000002</v>
+        <v>-935.69</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -513,7 +513,7 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>48.847999999999999</v>
+        <v>-790.452</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
@@ -533,15 +533,15 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>-948.92700000000002</v>
+        <v>376.89299999999997</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -553,15 +553,15 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>946.97400000000005</v>
+        <v>-871.66399999999999</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -573,15 +573,15 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-536.70699999999999</v>
+        <v>-647.51800000000003</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -593,21 +593,21 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>-774.13800000000003</v>
+        <v>-714.34</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
     </row>
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.2840000000000007</v>
+        <v>825.57600000000002</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -615,19 +615,19 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.17599999999999999</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">VLOOKUP(B10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>897.923</v>
+        <v>189.107</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -639,31 +639,31 @@
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-979.32299999999998</v>
+        <v>-302.87</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>498.55500000000001</v>
+        <v>829.6</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L10" t="str">
         <f ca="1">VLOOKUP(K10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="M10" s="6">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-686.28700000000003</v>
+        <v>-578.67700000000002</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -675,85 +675,85 @@
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>263.97399999999999</v>
+        <v>-614.05899999999997</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R10" t="str">
         <f ca="1">VLOOKUP(Q10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>163.54</v>
+        <v>-189.43799999999999</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>5.8999999999999997E-2</v>
+        <v>0.85199999999999998</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:C19" ca="1" si="5">VLOOKUP(B11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>592.29399999999998</v>
+        <v>447.03899999999999</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-851.779</v>
+        <v>907.47900000000004</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ref="I11:I19" ca="1" si="11">VLOOKUP(H11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-847.49599999999998</v>
+        <v>84.872</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:L19" ca="1" si="14">VLOOKUP(K11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-683.57899999999995</v>
+        <v>-635.572</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O19" ca="1" si="17">VLOOKUP(N11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-928.35900000000004</v>
+        <v>-895.56500000000005</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
@@ -765,73 +765,73 @@
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-770.98400000000004</v>
+        <v>290.47000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.68400000000000005</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>-451.35300000000001</v>
+        <v>472.50400000000002</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>-534.45100000000002</v>
+        <v>62.054000000000002</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>903.53800000000001</v>
+        <v>995.43899999999996</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>734.50699999999995</v>
+        <v>164.934</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>686.52099999999996</v>
+        <v>693.74800000000005</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
@@ -843,49 +843,49 @@
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>-721.79399999999998</v>
+        <v>-827.50400000000002</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.78900000000000003</v>
+        <v>0.72499999999999998</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>449.99200000000002</v>
+        <v>-325.505</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>-593.04999999999995</v>
+        <v>95.843999999999994</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>923.70799999999997</v>
+        <v>-423.38200000000001</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
@@ -897,37 +897,37 @@
       </c>
       <c r="M13" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-459.57299999999998</v>
+        <v>389.97500000000002</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>-978.31899999999996</v>
+        <v>-606.37400000000002</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>192.35400000000001</v>
+        <v>-154.03800000000001</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14399999999999999</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
@@ -939,7 +939,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>-133.678</v>
+        <v>91.674999999999997</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
@@ -951,19 +951,19 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>-560.76599999999996</v>
+        <v>295.87599999999998</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>710.50800000000004</v>
+        <v>49.476999999999997</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
@@ -975,7 +975,7 @@
       </c>
       <c r="M14" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-466.73399999999998</v>
+        <v>-675.245</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
@@ -987,73 +987,73 @@
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>233.59200000000001</v>
+        <v>-914.41899999999998</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>-649.63199999999995</v>
+        <v>286.29300000000001</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.67500000000000004</v>
+        <v>1.2E-2</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>899.02200000000005</v>
+        <v>226.73</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>-808.42399999999998</v>
+        <v>941.65</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>-12.257</v>
+        <v>-506.93700000000001</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>685.63099999999997</v>
+        <v>947.19299999999998</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
@@ -1065,103 +1065,103 @@
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>222.697</v>
+        <v>-172.15100000000001</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>-888.00300000000004</v>
+        <v>-724.75300000000004</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.61099999999999999</v>
+        <v>0.48</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>-827.53300000000002</v>
+        <v>36.398000000000003</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>-329.82400000000001</v>
+        <v>-498.37299999999999</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>309.995</v>
+        <v>-831.69299999999998</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-939.12300000000005</v>
+        <v>457.17099999999999</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>938.55200000000002</v>
+        <v>336.69499999999999</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>-535.93100000000004</v>
+        <v>359.94</v>
       </c>
     </row>
     <row r="17" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.38</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
@@ -1173,7 +1173,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>444.41399999999999</v>
+        <v>409.04399999999998</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
@@ -1185,31 +1185,31 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>373.029</v>
+        <v>458.06799999999998</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>-220.96299999999999</v>
+        <v>27.774999999999999</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>649.36500000000001</v>
+        <v>333.08699999999999</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>-180.09200000000001</v>
+        <v>596.62699999999995</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
@@ -1233,25 +1233,25 @@
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>-562.07500000000005</v>
+        <v>-677.81799999999998</v>
       </c>
     </row>
     <row r="18" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.75600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>-770.01499999999999</v>
+        <v>598.29600000000005</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
@@ -1263,19 +1263,19 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>-276.62799999999999</v>
+        <v>966.65</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>953.42600000000004</v>
+        <v>-730.26800000000003</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
@@ -1287,37 +1287,37 @@
       </c>
       <c r="M18" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>486.91199999999998</v>
+        <v>-758.32</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>-105.758</v>
+        <v>435.82</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>-700.99900000000002</v>
+        <v>-892.31100000000004</v>
       </c>
     </row>
     <row r="19" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>8.7999999999999995E-2</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
@@ -1329,19 +1329,19 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>274.30099999999999</v>
+        <v>-987.56299999999999</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>-477.315</v>
+        <v>64.305999999999997</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
@@ -1353,43 +1353,43 @@
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>127.00700000000001</v>
+        <v>-202.36799999999999</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>605.02800000000002</v>
+        <v>790.3</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>897.23099999999999</v>
+        <v>93.703000000000003</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>357.23</v>
+        <v>309.01</v>
       </c>
     </row>
     <row r="20" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Make clear button more compreshensive
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -490,15 +490,15 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-935.69</v>
+        <v>-918.31399999999996</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C1" t="str">
         <f ca="1">VLOOKUP(B1,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -513,15 +513,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-790.452</v>
+        <v>166.393</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -533,15 +533,15 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>376.89299999999997</v>
+        <v>167.56399999999999</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -553,15 +553,15 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>-871.66399999999999</v>
+        <v>361.57100000000003</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -573,15 +573,15 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-647.51800000000003</v>
+        <v>-611.69100000000003</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -593,21 +593,21 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>-714.34</v>
+        <v>827.35199999999998</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
     </row>
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>825.57600000000002</v>
+        <v>-703.06200000000001</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -615,43 +615,43 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.91900000000000004</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">VLOOKUP(B10,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>189.107</v>
+        <v>-22.021999999999998</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(E10,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-302.87</v>
+        <v>-336.18400000000003</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>829.6</v>
+        <v>-835.01499999999999</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
@@ -663,61 +663,61 @@
       </c>
       <c r="M10" s="6">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-578.67700000000002</v>
+        <v>-860.06100000000004</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O10" t="str">
         <f ca="1">VLOOKUP(N10,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-614.05899999999997</v>
+        <v>-551.78</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10" t="str">
         <f ca="1">VLOOKUP(Q10,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-189.43799999999999</v>
+        <v>965.12599999999998</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.85199999999999998</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:C19" ca="1" si="5">VLOOKUP(B11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>447.03899999999999</v>
+        <v>-15.007999999999999</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" ref="F11:F19" ca="1" si="8">VLOOKUP(E11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>907.47900000000004</v>
+        <v>848.73199999999997</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
@@ -729,163 +729,163 @@
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>84.872</v>
+        <v>-571.75</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:L19" ca="1" si="14">VLOOKUP(K11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-635.572</v>
+        <v>697.90300000000002</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O19" ca="1" si="17">VLOOKUP(N11,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-895.56500000000005</v>
+        <v>-624.30600000000004</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ref="R11:R19" ca="1" si="20">VLOOKUP(Q11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>290.47000000000003</v>
+        <v>-595.89599999999996</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.14499999999999999</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>472.50400000000002</v>
+        <v>-71.034000000000006</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>62.054000000000002</v>
+        <v>-894.96600000000001</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>995.43899999999996</v>
+        <v>-806.19600000000003</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>164.934</v>
+        <v>-373.279</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>693.74800000000005</v>
+        <v>712.08299999999997</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>-827.50400000000002</v>
+        <v>-646.97699999999998</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.72499999999999998</v>
+        <v>0.371</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>-325.505</v>
+        <v>315.596</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>95.843999999999994</v>
+        <v>500.28300000000002</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>-423.38200000000001</v>
+        <v>-54.351999999999997</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
@@ -897,7 +897,7 @@
       </c>
       <c r="M13" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>389.97500000000002</v>
+        <v>-693.54200000000003</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
@@ -909,25 +909,25 @@
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>-606.37400000000002</v>
+        <v>-774.27300000000002</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>-154.03800000000001</v>
+        <v>-240.864</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>9.0999999999999998E-2</v>
+        <v>0.621</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
@@ -939,7 +939,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>91.674999999999997</v>
+        <v>939.10400000000004</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
@@ -951,73 +951,73 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>295.87599999999998</v>
+        <v>450.96699999999998</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>49.476999999999997</v>
+        <v>-58.055999999999997</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-675.245</v>
+        <v>461.65199999999999</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>-914.41899999999998</v>
+        <v>897.096</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>286.29300000000001</v>
+        <v>529.46500000000003</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>1.2E-2</v>
+        <v>0.218</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>226.73</v>
+        <v>-117.02</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
@@ -1029,85 +1029,85 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>941.65</v>
+        <v>-614.54999999999995</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>-506.93700000000001</v>
+        <v>87.106999999999999</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>947.19299999999998</v>
+        <v>205.191</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>-172.15100000000001</v>
+        <v>234.703</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>-724.75300000000004</v>
+        <v>-182.994</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.48</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>36.398000000000003</v>
+        <v>-726.89</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>-498.37299999999999</v>
+        <v>453.82499999999999</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
@@ -1119,85 +1119,85 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>-831.69299999999998</v>
+        <v>884.38</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>457.17099999999999</v>
+        <v>123.38500000000001</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>336.69499999999999</v>
+        <v>-768.28300000000002</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>359.94</v>
+        <v>-751.23900000000003</v>
       </c>
     </row>
     <row r="17" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.13600000000000001</v>
+        <v>0.59299999999999997</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>409.04399999999998</v>
+        <v>749.149</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>458.06799999999998</v>
+        <v>-798.726</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>27.774999999999999</v>
+        <v>421.77600000000001</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
@@ -1209,19 +1209,19 @@
       </c>
       <c r="M17" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>333.08699999999999</v>
+        <v>-339.99099999999999</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>596.62699999999995</v>
+        <v>905.91300000000001</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
@@ -1233,25 +1233,25 @@
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>-677.81799999999998</v>
+        <v>931.01599999999996</v>
       </c>
     </row>
     <row r="18" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.6</v>
+        <v>0.97199999999999998</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>598.29600000000005</v>
+        <v>655.16800000000001</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
@@ -1263,43 +1263,43 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>966.65</v>
+        <v>-527.19000000000005</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>-730.26800000000003</v>
+        <v>735.54899999999998</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-758.32</v>
+        <v>683.46</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O18" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>435.82</v>
+        <v>-820.56799999999998</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
@@ -1311,61 +1311,61 @@
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>-892.31100000000004</v>
+        <v>35.548000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.53100000000000003</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>-987.56299999999999</v>
+        <v>-9.9770000000000003</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>64.305999999999997</v>
+        <v>-173.57599999999999</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>-202.36799999999999</v>
+        <v>-195.96700000000001</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>790.3</v>
+        <v>985.70899999999995</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
@@ -1377,19 +1377,19 @@
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>93.703000000000003</v>
+        <v>-836.92899999999997</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>309.01</v>
+        <v>-398.73700000000002</v>
       </c>
     </row>
     <row r="20" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
refactor for math.js -- not done
</commit_message>
<xml_diff>
--- a/other/Tests.xlsx
+++ b/other/Tests.xlsx
@@ -458,7 +458,7 @@
   <dimension ref="A1:AA38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -490,15 +490,15 @@
     <row r="1" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-918.31399999999996</v>
+        <v>-952.84900000000005</v>
       </c>
       <c r="B1">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C1" t="str">
         <f ca="1">VLOOKUP(B1,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
@@ -513,15 +513,15 @@
     <row r="2" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A7" ca="1" si="0">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>166.393</v>
+        <v>-724.27300000000002</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B6" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C6" ca="1" si="2">VLOOKUP(B2,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -533,15 +533,15 @@
     <row r="3" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>167.56399999999999</v>
+        <v>41.771000000000001</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="H3">
         <v>2</v>
@@ -553,7 +553,7 @@
     <row r="4" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>361.57100000000003</v>
+        <v>347.15600000000001</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
@@ -573,15 +573,15 @@
     <row r="5" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>-611.69100000000003</v>
+        <v>-215.53100000000001</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="H5">
         <v>4</v>
@@ -593,7 +593,7 @@
     <row r="6" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>827.35199999999998</v>
+        <v>-767.96500000000003</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
@@ -607,7 +607,7 @@
     <row r="7" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>-703.06200000000001</v>
+        <v>632.26199999999994</v>
       </c>
     </row>
     <row r="8" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25"/>
@@ -615,97 +615,97 @@
     <row r="10" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f ca="1">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.55200000000000005</v>
+        <v>0.186</v>
       </c>
       <c r="B10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="str">
         <f ca="1">VLOOKUP(B10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="D10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-22.021999999999998</v>
+        <v>-976.07299999999998</v>
       </c>
       <c r="E10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
         <f ca="1">VLOOKUP(E10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="G10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-336.18400000000003</v>
+        <v>314.02499999999998</v>
       </c>
       <c r="H10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I10" t="str">
         <f ca="1">VLOOKUP(H10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>divide</v>
       </c>
       <c r="J10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-835.01499999999999</v>
+        <v>77.823999999999998</v>
       </c>
       <c r="K10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L10" t="str">
         <f ca="1">VLOOKUP(K10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="M10" s="6">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-860.06100000000004</v>
+        <v>-861.16099999999994</v>
       </c>
       <c r="N10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O10" t="str">
         <f ca="1">VLOOKUP(N10,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="P10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-551.78</v>
+        <v>649.66999999999996</v>
       </c>
       <c r="Q10">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R10" t="str">
         <f ca="1">VLOOKUP(Q10,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S10">
         <f ca="1">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>965.12599999999998</v>
+        <v>243.75700000000001</v>
       </c>
     </row>
     <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ref="A11:A19" ca="1" si="3">(RANDBETWEEN(-0.5,0.01)+(ROUND((RAND()),3)))</f>
-        <v>0.44500000000000001</v>
+        <v>0.56899999999999995</v>
       </c>
       <c r="B11">
         <f t="shared" ref="B11:B19" ca="1" si="4">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ref="C11:C19" ca="1" si="5">VLOOKUP(B11,$H$1:$I$5,2,FALSE)</f>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" ca="1" si="6">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-15.007999999999999</v>
+        <v>-150.422</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" ca="1" si="7">RANDBETWEEN(1,4)</f>
@@ -717,139 +717,139 @@
       </c>
       <c r="G11">
         <f t="shared" ref="G11:G19" ca="1" si="9">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>848.73199999999997</v>
+        <v>495.26</v>
       </c>
       <c r="H11">
         <f t="shared" ref="H11:H19" ca="1" si="10">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" t="str">
         <f t="shared" ref="I11:I19" ca="1" si="11">VLOOKUP(H11,$H$1:$I$5,2,FALSE)</f>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="J11">
         <f t="shared" ref="J11:J19" ca="1" si="12">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-571.75</v>
+        <v>56.723999999999997</v>
       </c>
       <c r="K11">
         <f t="shared" ref="K11:K19" ca="1" si="13">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ref="L11:L19" ca="1" si="14">VLOOKUP(K11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="M11" s="6">
         <f t="shared" ref="M11:M19" ca="1" si="15">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>697.90300000000002</v>
+        <v>-447.97199999999998</v>
       </c>
       <c r="N11">
         <f t="shared" ref="N11:N19" ca="1" si="16">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O11" t="str">
         <f t="shared" ref="O11:O19" ca="1" si="17">VLOOKUP(N11,$H$1:$I$5,2,FALSE)</f>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="P11">
         <f t="shared" ref="P11:P19" ca="1" si="18">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-624.30600000000004</v>
+        <v>-766.35599999999999</v>
       </c>
       <c r="Q11">
         <f t="shared" ref="Q11:Q19" ca="1" si="19">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ref="R11:R19" ca="1" si="20">VLOOKUP(Q11,$H$1:$I$5,2,FALSE)</f>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="S11">
         <f t="shared" ref="S11:S19" ca="1" si="21">(RANDBETWEEN(-1000,1000)+(ROUND((RAND()),3)))</f>
-        <v>-595.89599999999996</v>
+        <v>740.28200000000004</v>
       </c>
     </row>
     <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="3"/>
-        <v>0.98399999999999999</v>
+        <v>0.67</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="6"/>
-        <v>-71.034000000000006</v>
+        <v>-728.62900000000002</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="9"/>
-        <v>-894.96600000000001</v>
+        <v>-884.73900000000003</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="12"/>
-        <v>-806.19600000000003</v>
+        <v>-798.13199999999995</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="M12" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-373.279</v>
+        <v>-925.23500000000001</v>
       </c>
       <c r="N12">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O12" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="P12">
         <f t="shared" ca="1" si="18"/>
-        <v>712.08299999999997</v>
+        <v>379.822</v>
       </c>
       <c r="Q12">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S12">
         <f t="shared" ca="1" si="21"/>
-        <v>-646.97699999999998</v>
+        <v>984.94</v>
       </c>
     </row>
     <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="3"/>
-        <v>0.371</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="4"/>
@@ -861,31 +861,31 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="6"/>
-        <v>315.596</v>
+        <v>643.274</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="9"/>
-        <v>500.28300000000002</v>
+        <v>988.65099999999995</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I13" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="12"/>
-        <v>-54.351999999999997</v>
+        <v>-925.79300000000001</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="13"/>
@@ -897,19 +897,19 @@
       </c>
       <c r="M13" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-693.54200000000003</v>
+        <v>-263.49599999999998</v>
       </c>
       <c r="N13">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="O13" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="P13">
         <f t="shared" ca="1" si="18"/>
-        <v>-774.27300000000002</v>
+        <v>-775.50300000000004</v>
       </c>
       <c r="Q13">
         <f t="shared" ca="1" si="19"/>
@@ -921,25 +921,25 @@
       </c>
       <c r="S13">
         <f t="shared" ca="1" si="21"/>
-        <v>-240.864</v>
+        <v>115.935</v>
       </c>
     </row>
     <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="3"/>
-        <v>0.621</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="6"/>
-        <v>939.10400000000004</v>
+        <v>612.72299999999996</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="7"/>
@@ -951,217 +951,217 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="9"/>
-        <v>450.96699999999998</v>
+        <v>-853.36599999999999</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="12"/>
-        <v>-58.055999999999997</v>
+        <v>516.68299999999999</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="M14" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>461.65199999999999</v>
+        <v>-626.37699999999995</v>
       </c>
       <c r="N14">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O14" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="P14">
         <f t="shared" ca="1" si="18"/>
-        <v>897.096</v>
+        <v>-627.66300000000001</v>
       </c>
       <c r="Q14">
         <f t="shared" ca="1" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="S14">
         <f t="shared" ca="1" si="21"/>
-        <v>529.46500000000003</v>
+        <v>432.01299999999998</v>
       </c>
     </row>
     <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="3"/>
-        <v>0.218</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="6"/>
-        <v>-117.02</v>
+        <v>-712.79300000000001</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="9"/>
-        <v>-614.54999999999995</v>
+        <v>874.17399999999998</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I15" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="12"/>
-        <v>87.106999999999999</v>
+        <v>763.74900000000002</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="M15" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>205.191</v>
+        <v>822.81200000000001</v>
       </c>
       <c r="N15">
         <f t="shared" ca="1" si="16"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O15" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>times</v>
+        <v>add</v>
       </c>
       <c r="P15">
         <f t="shared" ca="1" si="18"/>
-        <v>234.703</v>
+        <v>-796.16700000000003</v>
       </c>
       <c r="Q15">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S15">
         <f t="shared" ca="1" si="21"/>
-        <v>-182.994</v>
+        <v>-788.495</v>
       </c>
     </row>
     <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="3"/>
-        <v>0.92400000000000004</v>
+        <v>0.78</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="6"/>
-        <v>-726.89</v>
+        <v>-956.86800000000005</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="9"/>
-        <v>453.82499999999999</v>
+        <v>-133.24</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="12"/>
-        <v>884.38</v>
+        <v>685.18</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>times</v>
       </c>
       <c r="M16" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>123.38500000000001</v>
+        <v>-232.52600000000001</v>
       </c>
       <c r="N16">
         <f t="shared" ca="1" si="16"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O16" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>minus</v>
+        <v>add</v>
       </c>
       <c r="P16">
         <f t="shared" ca="1" si="18"/>
-        <v>-768.28300000000002</v>
+        <v>697.20399999999995</v>
       </c>
       <c r="Q16">
         <f t="shared" ca="1" si="19"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="S16">
         <f t="shared" ca="1" si="21"/>
-        <v>-751.23900000000003</v>
+        <v>-141.09899999999999</v>
       </c>
     </row>
     <row r="17" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="3"/>
-        <v>0.59299999999999997</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="4"/>
@@ -1173,121 +1173,121 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="6"/>
-        <v>749.149</v>
+        <v>-920.79700000000003</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="7"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="9"/>
-        <v>-798.726</v>
+        <v>535.42700000000002</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I17" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="12"/>
-        <v>421.77600000000001</v>
+        <v>462.791</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="M17" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>-339.99099999999999</v>
+        <v>-747.78899999999999</v>
       </c>
       <c r="N17">
         <f t="shared" ca="1" si="16"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O17" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="P17">
         <f t="shared" ca="1" si="18"/>
-        <v>905.91300000000001</v>
+        <v>475.916</v>
       </c>
       <c r="Q17">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="S17">
         <f t="shared" ca="1" si="21"/>
-        <v>931.01599999999996</v>
+        <v>-608.06700000000001</v>
       </c>
     </row>
     <row r="18" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="3"/>
-        <v>0.97199999999999998</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="6"/>
-        <v>655.16800000000001</v>
+        <v>-204.56700000000001</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>add</v>
+        <v>minus</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="9"/>
-        <v>-527.19000000000005</v>
+        <v>-541.87900000000002</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>divide</v>
+        <v>minus</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="12"/>
-        <v>735.54899999999998</v>
+        <v>-183.40600000000001</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="13"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>add</v>
+        <v>divide</v>
       </c>
       <c r="M18" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>683.46</v>
+        <v>313.97500000000002</v>
       </c>
       <c r="N18">
         <f t="shared" ca="1" si="16"/>
@@ -1299,97 +1299,97 @@
       </c>
       <c r="P18">
         <f t="shared" ca="1" si="18"/>
-        <v>-820.56799999999998</v>
+        <v>-769.18499999999995</v>
       </c>
       <c r="Q18">
         <f t="shared" ca="1" si="19"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="S18">
         <f t="shared" ca="1" si="21"/>
-        <v>35.548000000000002</v>
+        <v>-72.075000000000003</v>
       </c>
     </row>
     <row r="19" spans="1:27" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.85599999999999998</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>times</v>
+        <v>divide</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="6"/>
-        <v>-9.9770000000000003</v>
+        <v>315.64</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>times</v>
+        <v>minus</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="9"/>
-        <v>-173.57599999999999</v>
+        <v>-801.80100000000004</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I19" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>minus</v>
+        <v>times</v>
       </c>
       <c r="J19">
         <f t="shared" ca="1" si="12"/>
-        <v>-195.96700000000001</v>
+        <v>-155.828</v>
       </c>
       <c r="K19">
         <f t="shared" ca="1" si="13"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>divide</v>
+        <v>add</v>
       </c>
       <c r="M19" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>985.70899999999995</v>
+        <v>674.75699999999995</v>
       </c>
       <c r="N19">
         <f t="shared" ca="1" si="16"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O19" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="P19">
         <f t="shared" ca="1" si="18"/>
-        <v>-836.92899999999997</v>
+        <v>48.517000000000003</v>
       </c>
       <c r="Q19">
         <f t="shared" ca="1" si="19"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R19" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>divide</v>
+        <v>times</v>
       </c>
       <c r="S19">
         <f t="shared" ca="1" si="21"/>
-        <v>-398.73700000000002</v>
+        <v>231.066</v>
       </c>
     </row>
     <row r="20" spans="1:27" collapsed="1" x14ac:dyDescent="0.25">

</xml_diff>